<commit_message>
Discussion of WWDT post
</commit_message>
<xml_diff>
--- a/assets/img/WWDT/experimental_data.xlsx
+++ b/assets/img/WWDT/experimental_data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timothyweng/TimothyWeng.github.io/assets/img/WWDT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BB5C6B-FAAA-AE44-BEA1-F5348E72C242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059603D0-9101-044D-943D-56287EC2B451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pre" sheetId="8" r:id="rId1"/>
+    <sheet name="Main" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>TBT</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,6 +40,10 @@
   </si>
   <si>
     <t>CTL-slow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -88,10 +93,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -309,7 +315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F70F8833-2086-EC43-A781-C2149A5C4BB7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+    <sheetView zoomScale="173" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -360,4 +366,144 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2ED18EB-C0AA-4C4A-AD24-3AA013855D89}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>263</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="3"/>
+      <c r="B3">
+        <v>275</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="3"/>
+      <c r="B4">
+        <v>310</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="3"/>
+      <c r="B5">
+        <v>315</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="3"/>
+      <c r="B6">
+        <v>360</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="3"/>
+      <c r="B7">
+        <v>372</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>187</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.20649999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="3"/>
+      <c r="B9">
+        <v>190</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="3"/>
+      <c r="B10">
+        <v>268</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="3"/>
+      <c r="B11">
+        <v>273</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
+      <c r="B12">
+        <v>320</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.22699999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="3"/>
+      <c r="B13">
+        <v>328</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A13"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>